<commit_message>
controllo  materiali macchine cucito
</commit_message>
<xml_diff>
--- a/magazzino2019.xlsx
+++ b/magazzino2019.xlsx
@@ -1166,8 +1166,8 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A73" activeCellId="0" sqref="A73"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C148" activeCellId="0" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5114,14 +5114,14 @@
         <v>42</v>
       </c>
       <c r="F145" s="28" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G145" s="29" t="n">
         <v>2.2</v>
       </c>
       <c r="H145" s="16" t="n">
         <f aca="false">F145*G145</f>
-        <v>112.2</v>
+        <v>110</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5135,14 +5135,14 @@
         <v>42</v>
       </c>
       <c r="F146" s="28" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G146" s="29" t="n">
         <v>5.5</v>
       </c>
       <c r="H146" s="16" t="n">
         <f aca="false">F146*G146</f>
-        <v>203.5</v>
+        <v>209</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5156,14 +5156,14 @@
         <v>42</v>
       </c>
       <c r="F147" s="28" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G147" s="29" t="n">
         <v>0.4</v>
       </c>
       <c r="H147" s="16" t="n">
         <f aca="false">F147*G147</f>
-        <v>22.8</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5198,14 +5198,14 @@
         <v>42</v>
       </c>
       <c r="F149" s="28" t="n">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G149" s="29" t="n">
         <v>1.1</v>
       </c>
       <c r="H149" s="16" t="n">
         <f aca="false">F149*G149</f>
-        <v>45.1</v>
+        <v>57.2</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5240,14 +5240,14 @@
         <v>42</v>
       </c>
       <c r="F151" s="28" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G151" s="29" t="n">
         <v>2.85</v>
       </c>
       <c r="H151" s="16" t="n">
         <f aca="false">F151*G151</f>
-        <v>125.4</v>
+        <v>131.1</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5261,14 +5261,14 @@
         <v>42</v>
       </c>
       <c r="F152" s="28" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G152" s="29" t="n">
         <v>3.4</v>
       </c>
       <c r="H152" s="16" t="n">
         <f aca="false">F152*G152</f>
-        <v>125.8</v>
+        <v>122.4</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5383,7 +5383,7 @@
     <row r="158" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H158" s="44" t="n">
         <f aca="false">SUM(H3:H157)</f>
-        <v>20182.18</v>
+        <v>20199.48</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
variazione per prelievo  magazzino 12/3
</commit_message>
<xml_diff>
--- a/magazzino2019.xlsx
+++ b/magazzino2019.xlsx
@@ -1166,8 +1166,8 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C148" activeCellId="0" sqref="C148"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C115" activeCellId="0" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4345,14 +4345,14 @@
         <v>42</v>
       </c>
       <c r="F112" s="25" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G112" s="20" t="n">
         <v>2.5</v>
       </c>
       <c r="H112" s="16" t="n">
         <f aca="false">F112*G112</f>
-        <v>87.5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5383,7 +5383,7 @@
     <row r="158" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H158" s="44" t="n">
         <f aca="false">SUM(H3:H157)</f>
-        <v>20199.48</v>
+        <v>20196.98</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
prima del cambio distro 27 marzo
</commit_message>
<xml_diff>
--- a/magazzino2019.xlsx
+++ b/magazzino2019.xlsx
@@ -1166,8 +1166,8 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A105" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A117" activeCellId="0" sqref="A117"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2617,14 +2617,14 @@
         <v>63</v>
       </c>
       <c r="F37" s="25" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="G37" s="20" t="n">
         <v>2.6</v>
       </c>
       <c r="H37" s="16" t="n">
         <f aca="false">F37*G37</f>
-        <v>130</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4057,14 +4057,14 @@
         <v>42</v>
       </c>
       <c r="F100" s="25" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G100" s="38" t="n">
         <v>3.45</v>
       </c>
       <c r="H100" s="37" t="n">
         <f aca="false">F100*G100</f>
-        <v>296.7</v>
+        <v>293.25</v>
       </c>
       <c r="I100" s="40"/>
     </row>
@@ -4105,14 +4105,14 @@
         <v>42</v>
       </c>
       <c r="F102" s="25" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G102" s="38" t="n">
         <v>4.8</v>
       </c>
       <c r="H102" s="37" t="n">
         <f aca="false">F102*G102</f>
-        <v>86.4</v>
+        <v>0</v>
       </c>
       <c r="I102" s="40"/>
     </row>
@@ -4272,14 +4272,14 @@
         <v>42</v>
       </c>
       <c r="F109" s="25" t="n">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G109" s="38" t="n">
         <v>3.1</v>
       </c>
       <c r="H109" s="37" t="n">
         <f aca="false">F109*G109</f>
-        <v>496</v>
+        <v>492.9</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4449,14 +4449,14 @@
         <v>14</v>
       </c>
       <c r="F116" s="25" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G116" s="20" t="n">
         <v>2.4</v>
       </c>
       <c r="H116" s="16" t="n">
         <f aca="false">F116*G116</f>
-        <v>144</v>
+        <v>72</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5383,7 +5383,7 @@
     <row r="158" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H158" s="44" t="n">
         <f aca="false">SUM(H3:H157)</f>
-        <v>19418.61</v>
+        <v>19188.66</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>